<commit_message>
Updated data for multiple register.
</commit_message>
<xml_diff>
--- a/src/main/java/com/tutorialsninja/qa/testData/ExelData.xlsx
+++ b/src/main/java/com/tutorialsninja/qa/testData/ExelData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium4\TutorialsNinjaProject\src\main\java\com\tutorialsninja\qa\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\git\TutorialsNinja\src\main\java\com\tutorialsninja\qa\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2AF1EA0-BE97-4A34-A0EE-DBA1606EFC8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4555F7-3A3A-4C04-A7D9-05470CF7FD0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{F31AA47B-6E34-44A1-9FC5-18B13BFEB8BA}"/>
   </bookViews>
@@ -67,10 +67,10 @@
     <t>sdfau</t>
   </si>
   <si>
-    <t>task123@gmail.com</t>
-  </si>
-  <si>
-    <t>bdvbasydbabw@gmail.com</t>
+    <t>bt6g7h3b4@gmail.com</t>
+  </si>
+  <si>
+    <t>t5h8d4r6v8@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -485,7 +485,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -523,7 +523,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2">
         <v>4567893218</v>
@@ -543,7 +543,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3">
         <v>7536982418</v>

</xml_diff>

<commit_message>
New data for POI.
</commit_message>
<xml_diff>
--- a/src/main/java/com/tutorialsninja/qa/testData/ExelData.xlsx
+++ b/src/main/java/com/tutorialsninja/qa/testData/ExelData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium4\TutorialsNinjaProject\src\main\java\com\tutorialsninja\qa\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7fd51957c477b087/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2AF1EA0-BE97-4A34-A0EE-DBA1606EFC8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{5E7B15B5-7289-4037-9141-0249AF48651B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC841362-88A2-4076-8A27-824887BD3F02}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{F31AA47B-6E34-44A1-9FC5-18B13BFEB8BA}"/>
   </bookViews>
@@ -67,10 +67,10 @@
     <t>sdfau</t>
   </si>
   <si>
-    <t>task123@gmail.com</t>
-  </si>
-  <si>
-    <t>bdvbasydbabw@gmail.com</t>
+    <t>dksjbbdk123vb@gmail.com</t>
+  </si>
+  <si>
+    <t>tanuhsd456ye@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -485,7 +485,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -523,7 +523,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2">
         <v>4567893218</v>
@@ -543,7 +543,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3">
         <v>7536982418</v>

</xml_diff>